<commit_message>
Feat: Add feature export list students
</commit_message>
<xml_diff>
--- a/public/examples/users.xlsx
+++ b/public/examples/users.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Họ và Tên</t>
   </si>
@@ -51,15 +51,9 @@
     <t>Giới tính</t>
   </si>
   <si>
-    <t>htuanqn@12</t>
-  </si>
-  <si>
     <t>Phạm Hoàng Tuấn</t>
   </si>
   <si>
-    <t>tuanhoang@vlog.com</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -75,7 +69,19 @@
     <t>0812665001</t>
   </si>
   <si>
-    <t>FPTAptech@MapLearn@Edu</t>
+    <t>fptaptech1</t>
+  </si>
+  <si>
+    <t>fptaptech2</t>
+  </si>
+  <si>
+    <t>fptaptech2@gmail.com</t>
+  </si>
+  <si>
+    <t>fptaptech1@gmail.com</t>
+  </si>
+  <si>
+    <t>Aptech#123</t>
   </si>
 </sst>
 </file>
@@ -454,18 +460,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.75" customWidth="1"/>
-    <col min="2" max="2" width="42.08203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="15.58203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.75" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" customWidth="1"/>
     <col min="5" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.4140625" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" customWidth="1"/>
@@ -507,42 +513,94 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="1">
         <v>2006</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2006</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" display="htuanqn@12"/>
+    <hyperlink ref="A3" r:id="rId2" display="htuanqn@12"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>